<commit_message>
Testing is almost done
</commit_message>
<xml_diff>
--- a/TestingMatrix.xlsx
+++ b/TestingMatrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="10">
   <si>
     <t>CSV</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Combination</t>
-  </si>
-  <si>
-    <t>test .txt or .xlsx input for presence points</t>
   </si>
 </sst>
 </file>
@@ -97,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,11 +154,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +182,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,53 +464,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.140625" style="9"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -512,22 +506,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="I6" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -545,21 +537,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
@@ -573,20 +567,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
         <v>3</v>
       </c>
@@ -600,20 +597,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
@@ -631,16 +631,19 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
         <v>3</v>
       </c>
@@ -658,16 +661,19 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
+      <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
@@ -685,16 +691,19 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
         <v>4</v>
       </c>
@@ -712,6 +721,7 @@
       <c r="A32" t="s">
         <v>2</v>
       </c>
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>